<commit_message>
OW-206 fixed update issue by upgrading OGM to 2.1.0 and using their indexing feature
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/NewExposures.xlsx
+++ b/valuation-app/src/test/resources/excel/NewExposures.xlsx
@@ -571,7 +571,7 @@
     <t xml:space="preserve">3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">DKK-CIBOR2-DKNA13</t>
+    <t xml:space="preserve">DKK-CIBOR-DKNA13</t>
   </si>
   <si>
     <t xml:space="preserve">HKD</t>
@@ -1163,58 +1163,57 @@
   </sheetPr>
   <dimension ref="A1:AU320"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB305" activeCellId="1" sqref="D2:D181 AB305"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI19" activeCellId="0" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43630,45 +43629,43 @@
   <dimension ref="A1:AH101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="1" sqref="D2:D181 K36"/>
+      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54134,57 +54131,55 @@
   <dimension ref="A1:AT101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA101" activeCellId="1" sqref="D2:D181 AA101"/>
+      <selection pane="topLeft" activeCell="AA101" activeCellId="0" sqref="AA101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67386,53 +67381,52 @@
   <dimension ref="A1:AP181"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D181"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-268 fixed notional sign
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/NewExposures.xlsx
+++ b/valuation-app/src/test/resources/excel/NewExposures.xlsx
@@ -748,7 +748,7 @@
     <t xml:space="preserve">SGSI</t>
   </si>
   <si>
-    <t xml:space="preserve">SGD-SOR-VWAP</t>
+    <t xml:space="preserve">SGD-SOR-Reuters</t>
   </si>
   <si>
     <t xml:space="preserve">SGX</t>
@@ -1163,57 +1163,58 @@
   </sheetPr>
   <dimension ref="A1:AU320"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI19" activeCellId="0" sqref="AI19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI26" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43629,43 +43630,44 @@
   <dimension ref="A1:AH101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
+      <selection pane="topLeft" activeCell="K36" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54131,55 +54133,57 @@
   <dimension ref="A1:AT101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA101" activeCellId="0" sqref="AA101"/>
+      <selection pane="topLeft" activeCell="AA101" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 AA101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67380,53 +67384,54 @@
   </sheetPr>
   <dimension ref="A1:AP181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-6 improved performance by building trade list and save it in one request
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/NewExposures.xlsx
+++ b/valuation-app/src/test/resources/excel/NewExposures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19458" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19498" uniqueCount="343">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -1163,58 +1163,57 @@
   </sheetPr>
   <dimension ref="A1:AU320"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI26" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 AI26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43630,44 +43629,44 @@
   <dimension ref="A1:AH101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 K36"/>
+      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54132,58 +54131,57 @@
   </sheetPr>
   <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA101" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 AA101"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL4" activeCellId="0" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.4030612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.8010204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54786,8 +54784,8 @@
       <c r="Y5" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z5" s="0" t="n">
-        <v>400</v>
+      <c r="Z5" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA5" s="0" t="s">
         <v>142</v>
@@ -54822,8 +54820,8 @@
       <c r="AK5" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL5" s="0" t="n">
-        <v>400</v>
+      <c r="AL5" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN5" s="0" t="s">
         <v>64</v>
@@ -55438,8 +55436,8 @@
       <c r="Y10" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z10" s="0" t="n">
-        <v>400</v>
+      <c r="Z10" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA10" s="0" t="s">
         <v>142</v>
@@ -55474,8 +55472,8 @@
       <c r="AK10" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL10" s="0" t="n">
-        <v>400</v>
+      <c r="AL10" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN10" s="0" t="s">
         <v>64</v>
@@ -56090,8 +56088,8 @@
       <c r="Y15" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z15" s="0" t="n">
-        <v>400</v>
+      <c r="Z15" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA15" s="0" t="s">
         <v>142</v>
@@ -56126,8 +56124,8 @@
       <c r="AK15" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL15" s="0" t="n">
-        <v>400</v>
+      <c r="AL15" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN15" s="0" t="s">
         <v>64</v>
@@ -56742,8 +56740,8 @@
       <c r="Y20" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z20" s="0" t="n">
-        <v>400</v>
+      <c r="Z20" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA20" s="0" t="s">
         <v>142</v>
@@ -56778,8 +56776,8 @@
       <c r="AK20" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL20" s="0" t="n">
-        <v>400</v>
+      <c r="AL20" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN20" s="0" t="s">
         <v>64</v>
@@ -57394,8 +57392,8 @@
       <c r="Y25" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z25" s="0" t="n">
-        <v>400</v>
+      <c r="Z25" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA25" s="0" t="s">
         <v>142</v>
@@ -57430,8 +57428,8 @@
       <c r="AK25" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL25" s="0" t="n">
-        <v>400</v>
+      <c r="AL25" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN25" s="0" t="s">
         <v>64</v>
@@ -58046,8 +58044,8 @@
       <c r="Y30" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z30" s="0" t="n">
-        <v>400</v>
+      <c r="Z30" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA30" s="0" t="s">
         <v>142</v>
@@ -58082,8 +58080,8 @@
       <c r="AK30" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL30" s="0" t="n">
-        <v>400</v>
+      <c r="AL30" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN30" s="0" t="s">
         <v>64</v>
@@ -58698,8 +58696,8 @@
       <c r="Y35" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z35" s="0" t="n">
-        <v>400</v>
+      <c r="Z35" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA35" s="0" t="s">
         <v>142</v>
@@ -58734,8 +58732,8 @@
       <c r="AK35" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL35" s="0" t="n">
-        <v>400</v>
+      <c r="AL35" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN35" s="0" t="s">
         <v>64</v>
@@ -59350,8 +59348,8 @@
       <c r="Y40" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z40" s="0" t="n">
-        <v>400</v>
+      <c r="Z40" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA40" s="0" t="s">
         <v>142</v>
@@ -59386,8 +59384,8 @@
       <c r="AK40" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL40" s="0" t="n">
-        <v>400</v>
+      <c r="AL40" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN40" s="0" t="s">
         <v>64</v>
@@ -60002,8 +60000,8 @@
       <c r="Y45" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z45" s="0" t="n">
-        <v>400</v>
+      <c r="Z45" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA45" s="0" t="s">
         <v>142</v>
@@ -60038,8 +60036,8 @@
       <c r="AK45" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL45" s="0" t="n">
-        <v>400</v>
+      <c r="AL45" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN45" s="0" t="s">
         <v>64</v>
@@ -60654,8 +60652,8 @@
       <c r="Y50" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z50" s="0" t="n">
-        <v>400</v>
+      <c r="Z50" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA50" s="0" t="s">
         <v>142</v>
@@ -60690,8 +60688,8 @@
       <c r="AK50" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL50" s="0" t="n">
-        <v>400</v>
+      <c r="AL50" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN50" s="0" t="s">
         <v>64</v>
@@ -61306,8 +61304,8 @@
       <c r="Y55" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z55" s="0" t="n">
-        <v>400</v>
+      <c r="Z55" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA55" s="0" t="s">
         <v>142</v>
@@ -61342,8 +61340,8 @@
       <c r="AK55" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL55" s="0" t="n">
-        <v>400</v>
+      <c r="AL55" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN55" s="0" t="s">
         <v>64</v>
@@ -61958,8 +61956,8 @@
       <c r="Y60" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z60" s="0" t="n">
-        <v>400</v>
+      <c r="Z60" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA60" s="0" t="s">
         <v>142</v>
@@ -61994,8 +61992,8 @@
       <c r="AK60" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL60" s="0" t="n">
-        <v>400</v>
+      <c r="AL60" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN60" s="0" t="s">
         <v>64</v>
@@ -62610,8 +62608,8 @@
       <c r="Y65" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z65" s="0" t="n">
-        <v>400</v>
+      <c r="Z65" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA65" s="0" t="s">
         <v>142</v>
@@ -62646,8 +62644,8 @@
       <c r="AK65" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL65" s="0" t="n">
-        <v>400</v>
+      <c r="AL65" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN65" s="0" t="s">
         <v>64</v>
@@ -63262,8 +63260,8 @@
       <c r="Y70" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z70" s="0" t="n">
-        <v>400</v>
+      <c r="Z70" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA70" s="0" t="s">
         <v>142</v>
@@ -63298,8 +63296,8 @@
       <c r="AK70" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL70" s="0" t="n">
-        <v>400</v>
+      <c r="AL70" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN70" s="0" t="s">
         <v>64</v>
@@ -63914,8 +63912,8 @@
       <c r="Y75" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z75" s="0" t="n">
-        <v>400</v>
+      <c r="Z75" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA75" s="0" t="s">
         <v>142</v>
@@ -63950,8 +63948,8 @@
       <c r="AK75" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL75" s="0" t="n">
-        <v>400</v>
+      <c r="AL75" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN75" s="0" t="s">
         <v>64</v>
@@ -64566,8 +64564,8 @@
       <c r="Y80" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z80" s="0" t="n">
-        <v>400</v>
+      <c r="Z80" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA80" s="0" t="s">
         <v>142</v>
@@ -64602,8 +64600,8 @@
       <c r="AK80" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL80" s="0" t="n">
-        <v>400</v>
+      <c r="AL80" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN80" s="0" t="s">
         <v>64</v>
@@ -65218,8 +65216,8 @@
       <c r="Y85" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z85" s="0" t="n">
-        <v>400</v>
+      <c r="Z85" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA85" s="0" t="s">
         <v>142</v>
@@ -65254,8 +65252,8 @@
       <c r="AK85" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL85" s="0" t="n">
-        <v>400</v>
+      <c r="AL85" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN85" s="0" t="s">
         <v>64</v>
@@ -65870,8 +65868,8 @@
       <c r="Y90" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z90" s="0" t="n">
-        <v>400</v>
+      <c r="Z90" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA90" s="0" t="s">
         <v>142</v>
@@ -65906,8 +65904,8 @@
       <c r="AK90" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL90" s="0" t="n">
-        <v>400</v>
+      <c r="AL90" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN90" s="0" t="s">
         <v>64</v>
@@ -66522,8 +66520,8 @@
       <c r="Y95" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z95" s="0" t="n">
-        <v>400</v>
+      <c r="Z95" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA95" s="0" t="s">
         <v>142</v>
@@ -66558,8 +66556,8 @@
       <c r="AK95" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL95" s="0" t="n">
-        <v>400</v>
+      <c r="AL95" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN95" s="0" t="s">
         <v>64</v>
@@ -67174,8 +67172,8 @@
       <c r="Y100" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="Z100" s="0" t="n">
-        <v>400</v>
+      <c r="Z100" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AA100" s="0" t="s">
         <v>142</v>
@@ -67210,8 +67208,8 @@
       <c r="AK100" s="1" t="n">
         <v>44168</v>
       </c>
-      <c r="AL100" s="0" t="n">
-        <v>400</v>
+      <c r="AL100" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="AN100" s="0" t="s">
         <v>64</v>
@@ -67384,54 +67382,53 @@
   </sheetPr>
   <dimension ref="A1:AP181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="15" sqref="AE12:AE13 AE24:AE25 AE36:AE37 AE48:AE49 AE60:AE61 AE72:AE73 AE84:AE85 AE96:AE97 AE108:AE109 AE120:AE121 AE132:AE133 AE144:AE145 AE156:AE157 AE168:AE169 AE180:AE181 D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-6 more valuation fixes
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/NewExposures.xlsx
+++ b/valuation-app/src/test/resources/excel/NewExposures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19498" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19498" uniqueCount="340">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -1012,7 +1012,7 @@
     <t xml:space="preserve">0.07804</t>
   </si>
   <si>
-    <t xml:space="preserve">INR-MIBOR</t>
+    <t xml:space="preserve">INR-MIFOR</t>
   </si>
   <si>
     <t xml:space="preserve">1D</t>
@@ -1028,9 +1028,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.07476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INR-MIBOR-OIS-Swap Rate</t>
   </si>
   <si>
     <t xml:space="preserve">0.07612</t>
@@ -1157,58 +1154,57 @@
   </sheetPr>
   <dimension ref="A1:AU320"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P137" activeCellId="1" sqref="P122 P137"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z286" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P137" activeCellId="0" sqref="P137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43624,43 +43620,45 @@
   <dimension ref="A1:AH101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="1" sqref="P122 T6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.65816326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.4642857142857"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.9642857142857"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.4030612244898"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="23.8010204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54125,57 +54123,57 @@
   </sheetPr>
   <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL4" activeCellId="1" sqref="P122 AL4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.4030612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.8010204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67376,54 +67374,53 @@
   </sheetPr>
   <dimension ref="A1:AP181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P122" activeCellId="0" sqref="P122"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE90" activeCellId="0" sqref="AE90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68101,7 +68098,7 @@
         <v>59</v>
       </c>
       <c r="AE6" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF6" s="0" t="s">
         <v>330</v>
@@ -68196,7 +68193,7 @@
         <v>60</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y7" s="0" t="s">
         <v>62</v>
@@ -68217,7 +68214,7 @@
         <v>59</v>
       </c>
       <c r="AE7" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF7" s="0" t="s">
         <v>330</v>
@@ -68363,7 +68360,7 @@
         <v>12011167</v>
       </c>
       <c r="AP8" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68479,7 +68476,7 @@
         <v>12011168</v>
       </c>
       <c r="AP9" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68544,7 +68541,7 @@
         <v>60</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y10" s="0" t="s">
         <v>62</v>
@@ -68595,7 +68592,7 @@
         <v>12011169</v>
       </c>
       <c r="AP10" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68711,7 +68708,7 @@
         <v>12011170</v>
       </c>
       <c r="AP11" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68827,7 +68824,7 @@
         <v>12011171</v>
       </c>
       <c r="AP12" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68943,7 +68940,7 @@
         <v>12011172</v>
       </c>
       <c r="AP13" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69493,7 +69490,7 @@
         <v>59</v>
       </c>
       <c r="AE18" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF18" s="0" t="s">
         <v>330</v>
@@ -69588,7 +69585,7 @@
         <v>60</v>
       </c>
       <c r="X19" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y19" s="0" t="s">
         <v>62</v>
@@ -69609,7 +69606,7 @@
         <v>59</v>
       </c>
       <c r="AE19" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF19" s="0" t="s">
         <v>330</v>
@@ -69755,7 +69752,7 @@
         <v>12011167</v>
       </c>
       <c r="AP20" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69871,7 +69868,7 @@
         <v>12011168</v>
       </c>
       <c r="AP21" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69936,7 +69933,7 @@
         <v>60</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y22" s="0" t="s">
         <v>62</v>
@@ -69987,7 +69984,7 @@
         <v>12011169</v>
       </c>
       <c r="AP22" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70103,7 +70100,7 @@
         <v>12011170</v>
       </c>
       <c r="AP23" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70219,7 +70216,7 @@
         <v>12011171</v>
       </c>
       <c r="AP24" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70335,7 +70332,7 @@
         <v>12011172</v>
       </c>
       <c r="AP25" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70885,7 +70882,7 @@
         <v>59</v>
       </c>
       <c r="AE30" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF30" s="0" t="s">
         <v>330</v>
@@ -70980,7 +70977,7 @@
         <v>60</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y31" s="0" t="s">
         <v>62</v>
@@ -71001,7 +70998,7 @@
         <v>59</v>
       </c>
       <c r="AE31" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF31" s="0" t="s">
         <v>330</v>
@@ -71147,7 +71144,7 @@
         <v>12011167</v>
       </c>
       <c r="AP32" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71263,7 +71260,7 @@
         <v>12011168</v>
       </c>
       <c r="AP33" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71328,7 +71325,7 @@
         <v>60</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y34" s="0" t="s">
         <v>62</v>
@@ -71379,7 +71376,7 @@
         <v>12011169</v>
       </c>
       <c r="AP34" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71495,7 +71492,7 @@
         <v>12011170</v>
       </c>
       <c r="AP35" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71611,7 +71608,7 @@
         <v>12011171</v>
       </c>
       <c r="AP36" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71727,7 +71724,7 @@
         <v>12011172</v>
       </c>
       <c r="AP37" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -72277,7 +72274,7 @@
         <v>59</v>
       </c>
       <c r="AE42" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF42" s="0" t="s">
         <v>330</v>
@@ -72372,7 +72369,7 @@
         <v>60</v>
       </c>
       <c r="X43" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y43" s="0" t="s">
         <v>62</v>
@@ -72393,7 +72390,7 @@
         <v>59</v>
       </c>
       <c r="AE43" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF43" s="0" t="s">
         <v>330</v>
@@ -72539,7 +72536,7 @@
         <v>12011167</v>
       </c>
       <c r="AP44" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -72655,7 +72652,7 @@
         <v>12011168</v>
       </c>
       <c r="AP45" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -72720,7 +72717,7 @@
         <v>60</v>
       </c>
       <c r="X46" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y46" s="0" t="s">
         <v>62</v>
@@ -72771,7 +72768,7 @@
         <v>12011169</v>
       </c>
       <c r="AP46" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -72887,7 +72884,7 @@
         <v>12011170</v>
       </c>
       <c r="AP47" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73003,7 +73000,7 @@
         <v>12011171</v>
       </c>
       <c r="AP48" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73119,7 +73116,7 @@
         <v>12011172</v>
       </c>
       <c r="AP49" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73669,7 +73666,7 @@
         <v>59</v>
       </c>
       <c r="AE54" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF54" s="0" t="s">
         <v>330</v>
@@ -73764,7 +73761,7 @@
         <v>60</v>
       </c>
       <c r="X55" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y55" s="0" t="s">
         <v>62</v>
@@ -73785,7 +73782,7 @@
         <v>59</v>
       </c>
       <c r="AE55" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF55" s="0" t="s">
         <v>330</v>
@@ -73931,7 +73928,7 @@
         <v>12011167</v>
       </c>
       <c r="AP56" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74047,7 +74044,7 @@
         <v>12011168</v>
       </c>
       <c r="AP57" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74112,7 +74109,7 @@
         <v>60</v>
       </c>
       <c r="X58" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y58" s="0" t="s">
         <v>62</v>
@@ -74163,7 +74160,7 @@
         <v>12011169</v>
       </c>
       <c r="AP58" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74279,7 +74276,7 @@
         <v>12011170</v>
       </c>
       <c r="AP59" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74395,7 +74392,7 @@
         <v>12011171</v>
       </c>
       <c r="AP60" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74511,7 +74508,7 @@
         <v>12011172</v>
       </c>
       <c r="AP61" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75061,7 +75058,7 @@
         <v>59</v>
       </c>
       <c r="AE66" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF66" s="0" t="s">
         <v>330</v>
@@ -75156,7 +75153,7 @@
         <v>60</v>
       </c>
       <c r="X67" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y67" s="0" t="s">
         <v>62</v>
@@ -75177,7 +75174,7 @@
         <v>59</v>
       </c>
       <c r="AE67" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF67" s="0" t="s">
         <v>330</v>
@@ -75323,7 +75320,7 @@
         <v>12011167</v>
       </c>
       <c r="AP68" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75439,7 +75436,7 @@
         <v>12011168</v>
       </c>
       <c r="AP69" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75504,7 +75501,7 @@
         <v>60</v>
       </c>
       <c r="X70" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y70" s="0" t="s">
         <v>62</v>
@@ -75555,7 +75552,7 @@
         <v>12011169</v>
       </c>
       <c r="AP70" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75671,7 +75668,7 @@
         <v>12011170</v>
       </c>
       <c r="AP71" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75787,7 +75784,7 @@
         <v>12011171</v>
       </c>
       <c r="AP72" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75903,7 +75900,7 @@
         <v>12011172</v>
       </c>
       <c r="AP73" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76453,7 +76450,7 @@
         <v>59</v>
       </c>
       <c r="AE78" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF78" s="0" t="s">
         <v>330</v>
@@ -76548,7 +76545,7 @@
         <v>60</v>
       </c>
       <c r="X79" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y79" s="0" t="s">
         <v>62</v>
@@ -76569,7 +76566,7 @@
         <v>59</v>
       </c>
       <c r="AE79" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF79" s="0" t="s">
         <v>330</v>
@@ -76715,7 +76712,7 @@
         <v>12011167</v>
       </c>
       <c r="AP80" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76831,7 +76828,7 @@
         <v>12011168</v>
       </c>
       <c r="AP81" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76896,7 +76893,7 @@
         <v>60</v>
       </c>
       <c r="X82" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y82" s="0" t="s">
         <v>62</v>
@@ -76947,7 +76944,7 @@
         <v>12011169</v>
       </c>
       <c r="AP82" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -77063,7 +77060,7 @@
         <v>12011170</v>
       </c>
       <c r="AP83" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -77179,7 +77176,7 @@
         <v>12011171</v>
       </c>
       <c r="AP84" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -77295,7 +77292,7 @@
         <v>12011172</v>
       </c>
       <c r="AP85" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -77845,7 +77842,7 @@
         <v>59</v>
       </c>
       <c r="AE90" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF90" s="0" t="s">
         <v>330</v>
@@ -77940,7 +77937,7 @@
         <v>60</v>
       </c>
       <c r="X91" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y91" s="0" t="s">
         <v>62</v>
@@ -77961,7 +77958,7 @@
         <v>59</v>
       </c>
       <c r="AE91" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF91" s="0" t="s">
         <v>330</v>
@@ -78107,7 +78104,7 @@
         <v>12011167</v>
       </c>
       <c r="AP92" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78223,7 +78220,7 @@
         <v>12011168</v>
       </c>
       <c r="AP93" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78288,7 +78285,7 @@
         <v>60</v>
       </c>
       <c r="X94" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y94" s="0" t="s">
         <v>62</v>
@@ -78339,7 +78336,7 @@
         <v>12011169</v>
       </c>
       <c r="AP94" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78455,7 +78452,7 @@
         <v>12011170</v>
       </c>
       <c r="AP95" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78571,7 +78568,7 @@
         <v>12011171</v>
       </c>
       <c r="AP96" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -78687,7 +78684,7 @@
         <v>12011172</v>
       </c>
       <c r="AP97" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79237,7 +79234,7 @@
         <v>59</v>
       </c>
       <c r="AE102" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF102" s="0" t="s">
         <v>330</v>
@@ -79332,7 +79329,7 @@
         <v>60</v>
       </c>
       <c r="X103" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y103" s="0" t="s">
         <v>62</v>
@@ -79353,7 +79350,7 @@
         <v>59</v>
       </c>
       <c r="AE103" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF103" s="0" t="s">
         <v>330</v>
@@ -79499,7 +79496,7 @@
         <v>12011167</v>
       </c>
       <c r="AP104" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79615,7 +79612,7 @@
         <v>12011168</v>
       </c>
       <c r="AP105" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79680,7 +79677,7 @@
         <v>60</v>
       </c>
       <c r="X106" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y106" s="0" t="s">
         <v>62</v>
@@ -79731,7 +79728,7 @@
         <v>12011169</v>
       </c>
       <c r="AP106" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79847,7 +79844,7 @@
         <v>12011170</v>
       </c>
       <c r="AP107" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79963,7 +79960,7 @@
         <v>12011171</v>
       </c>
       <c r="AP108" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -80079,7 +80076,7 @@
         <v>12011172</v>
       </c>
       <c r="AP109" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -80629,7 +80626,7 @@
         <v>59</v>
       </c>
       <c r="AE114" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF114" s="0" t="s">
         <v>330</v>
@@ -80724,7 +80721,7 @@
         <v>60</v>
       </c>
       <c r="X115" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y115" s="0" t="s">
         <v>62</v>
@@ -80745,7 +80742,7 @@
         <v>59</v>
       </c>
       <c r="AE115" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF115" s="0" t="s">
         <v>330</v>
@@ -80891,7 +80888,7 @@
         <v>12011167</v>
       </c>
       <c r="AP116" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -81007,7 +81004,7 @@
         <v>12011168</v>
       </c>
       <c r="AP117" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -81072,7 +81069,7 @@
         <v>60</v>
       </c>
       <c r="X118" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y118" s="0" t="s">
         <v>62</v>
@@ -81123,7 +81120,7 @@
         <v>12011169</v>
       </c>
       <c r="AP118" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -81239,7 +81236,7 @@
         <v>12011170</v>
       </c>
       <c r="AP119" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -81355,7 +81352,7 @@
         <v>12011171</v>
       </c>
       <c r="AP120" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -81471,7 +81468,7 @@
         <v>12011172</v>
       </c>
       <c r="AP121" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82021,7 +82018,7 @@
         <v>59</v>
       </c>
       <c r="AE126" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF126" s="0" t="s">
         <v>330</v>
@@ -82116,7 +82113,7 @@
         <v>60</v>
       </c>
       <c r="X127" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y127" s="0" t="s">
         <v>62</v>
@@ -82137,7 +82134,7 @@
         <v>59</v>
       </c>
       <c r="AE127" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF127" s="0" t="s">
         <v>330</v>
@@ -82283,7 +82280,7 @@
         <v>12011167</v>
       </c>
       <c r="AP128" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82399,7 +82396,7 @@
         <v>12011168</v>
       </c>
       <c r="AP129" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82464,7 +82461,7 @@
         <v>60</v>
       </c>
       <c r="X130" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y130" s="0" t="s">
         <v>62</v>
@@ -82515,7 +82512,7 @@
         <v>12011169</v>
       </c>
       <c r="AP130" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82631,7 +82628,7 @@
         <v>12011170</v>
       </c>
       <c r="AP131" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82747,7 +82744,7 @@
         <v>12011171</v>
       </c>
       <c r="AP132" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -82863,7 +82860,7 @@
         <v>12011172</v>
       </c>
       <c r="AP133" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -83413,7 +83410,7 @@
         <v>59</v>
       </c>
       <c r="AE138" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF138" s="0" t="s">
         <v>330</v>
@@ -83508,7 +83505,7 @@
         <v>60</v>
       </c>
       <c r="X139" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y139" s="0" t="s">
         <v>62</v>
@@ -83529,7 +83526,7 @@
         <v>59</v>
       </c>
       <c r="AE139" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF139" s="0" t="s">
         <v>330</v>
@@ -83675,7 +83672,7 @@
         <v>12011167</v>
       </c>
       <c r="AP140" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -83791,7 +83788,7 @@
         <v>12011168</v>
       </c>
       <c r="AP141" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -83856,7 +83853,7 @@
         <v>60</v>
       </c>
       <c r="X142" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y142" s="0" t="s">
         <v>62</v>
@@ -83907,7 +83904,7 @@
         <v>12011169</v>
       </c>
       <c r="AP142" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -84023,7 +84020,7 @@
         <v>12011170</v>
       </c>
       <c r="AP143" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -84139,7 +84136,7 @@
         <v>12011171</v>
       </c>
       <c r="AP144" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -84255,7 +84252,7 @@
         <v>12011172</v>
       </c>
       <c r="AP145" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -84805,7 +84802,7 @@
         <v>59</v>
       </c>
       <c r="AE150" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF150" s="0" t="s">
         <v>330</v>
@@ -84900,7 +84897,7 @@
         <v>60</v>
       </c>
       <c r="X151" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y151" s="0" t="s">
         <v>62</v>
@@ -84921,7 +84918,7 @@
         <v>59</v>
       </c>
       <c r="AE151" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF151" s="0" t="s">
         <v>330</v>
@@ -85067,7 +85064,7 @@
         <v>12011167</v>
       </c>
       <c r="AP152" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -85183,7 +85180,7 @@
         <v>12011168</v>
       </c>
       <c r="AP153" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -85248,7 +85245,7 @@
         <v>60</v>
       </c>
       <c r="X154" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y154" s="0" t="s">
         <v>62</v>
@@ -85299,7 +85296,7 @@
         <v>12011169</v>
       </c>
       <c r="AP154" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -85415,7 +85412,7 @@
         <v>12011170</v>
       </c>
       <c r="AP155" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -85531,7 +85528,7 @@
         <v>12011171</v>
       </c>
       <c r="AP156" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -85647,7 +85644,7 @@
         <v>12011172</v>
       </c>
       <c r="AP157" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86197,7 +86194,7 @@
         <v>59</v>
       </c>
       <c r="AE162" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF162" s="0" t="s">
         <v>330</v>
@@ -86292,7 +86289,7 @@
         <v>60</v>
       </c>
       <c r="X163" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y163" s="0" t="s">
         <v>62</v>
@@ -86313,7 +86310,7 @@
         <v>59</v>
       </c>
       <c r="AE163" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF163" s="0" t="s">
         <v>330</v>
@@ -86459,7 +86456,7 @@
         <v>12011167</v>
       </c>
       <c r="AP164" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86575,7 +86572,7 @@
         <v>12011168</v>
       </c>
       <c r="AP165" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86640,7 +86637,7 @@
         <v>60</v>
       </c>
       <c r="X166" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y166" s="0" t="s">
         <v>62</v>
@@ -86691,7 +86688,7 @@
         <v>12011169</v>
       </c>
       <c r="AP166" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86807,7 +86804,7 @@
         <v>12011170</v>
       </c>
       <c r="AP167" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86923,7 +86920,7 @@
         <v>12011171</v>
       </c>
       <c r="AP168" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -87039,7 +87036,7 @@
         <v>12011172</v>
       </c>
       <c r="AP169" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -87589,7 +87586,7 @@
         <v>59</v>
       </c>
       <c r="AE174" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF174" s="0" t="s">
         <v>330</v>
@@ -87684,7 +87681,7 @@
         <v>60</v>
       </c>
       <c r="X175" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y175" s="0" t="s">
         <v>62</v>
@@ -87705,7 +87702,7 @@
         <v>59</v>
       </c>
       <c r="AE175" s="0" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AF175" s="0" t="s">
         <v>330</v>
@@ -87851,7 +87848,7 @@
         <v>12011167</v>
       </c>
       <c r="AP176" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -87967,7 +87964,7 @@
         <v>12011168</v>
       </c>
       <c r="AP177" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -88032,7 +88029,7 @@
         <v>60</v>
       </c>
       <c r="X178" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y178" s="0" t="s">
         <v>62</v>
@@ -88083,7 +88080,7 @@
         <v>12011169</v>
       </c>
       <c r="AP178" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -88199,7 +88196,7 @@
         <v>12011170</v>
       </c>
       <c r="AP179" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -88315,7 +88312,7 @@
         <v>12011171</v>
       </c>
       <c r="AP180" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -88431,7 +88428,7 @@
         <v>12011172</v>
       </c>
       <c r="AP181" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OW-248 externalized the graph data files into acuo-data
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/NewExposures.xlsx
+++ b/valuation-app/src/test/resources/excel/NewExposures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Portfolio ID</t>
   </si>
   <si>
-    <t xml:space="preserve">acc1</t>
+    <t xml:space="preserve">ACUOSG8745</t>
   </si>
   <si>
     <t xml:space="preserve">AUD</t>
@@ -1154,57 +1154,56 @@
   </sheetPr>
   <dimension ref="A1:AU320"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z286" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P137" activeCellId="0" sqref="P137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="48" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43625,40 +43624,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.07142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.5969387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.9642857142857"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.4030612244898"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="23.8010204081633"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54123,57 +54122,58 @@
   </sheetPr>
   <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.5969387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.4030612244898"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.8010204081633"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67374,53 +67374,52 @@
   </sheetPr>
   <dimension ref="A1:AP181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE90" activeCellId="0" sqref="AE90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>